<commit_message>
Correcting error in calculation of T* and adaptation analysis windows where windows were double the necessary length, due to miscalculation about frame rate (which is 1f/s instead of 2f/s)
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
+++ b/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49DB7DD-C56C-8747-89B8-53506D3292C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58946903-A180-1744-A714-1A0D2556FD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25120" yWindow="2380" windowWidth="23260" windowHeight="20020" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
+    <workbookView xWindow="0" yWindow="3860" windowWidth="35840" windowHeight="21940" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Tstar" sheetId="1" r:id="rId1"/>
@@ -497,9 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185A0AF1-AEF1-B74F-8EB8-314724BE975D}">
   <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71:F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +734,7 @@
         <v>21.2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>-0.90226152671895721</v>
@@ -995,7 +995,7 @@
         <v>21.7</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>-0.18936113009832178</v>
@@ -1024,7 +1024,7 @@
         <v>21.1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>-0.86368933181155483</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>15.75</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>16.5</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>14.9</v>
+        <v>15</v>
       </c>
       <c r="B27">
         <v>18.5</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>15.6</v>
+        <v>14.6</v>
       </c>
       <c r="B33">
         <v>17</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>23.1</v>
+        <v>15.4</v>
       </c>
       <c r="B47">
         <v>28.8</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>16.100000000000001</v>
+        <v>13.9</v>
       </c>
       <c r="B59">
         <v>26</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>16</v>
+        <v>15.4</v>
       </c>
       <c r="B63">
         <v>26</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>25.25</v>
+        <v>21.25</v>
       </c>
       <c r="B75">
         <v>28.6</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>22.6</v>
+        <v>20.6</v>
       </c>
       <c r="B79">
         <v>34</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>21.7</v>
+        <v>21</v>
       </c>
       <c r="B84">
         <v>34.1</v>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>37.35</v>
+        <v>30.8</v>
       </c>
       <c r="B86">
         <v>38.1</v>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>21.7</v>
+        <v>20.95</v>
       </c>
       <c r="B87">
         <v>40</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>25.2</v>
+        <v>24.4</v>
       </c>
       <c r="B97">
         <v>40.1</v>
@@ -3275,19 +3275,19 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C101">
-        <v>13.1</v>
+        <v>22.35</v>
       </c>
       <c r="E101">
-        <v>0.84273509813614655</v>
+        <v>0.84688402701513743</v>
       </c>
       <c r="G101">
-        <v>-12.612745716579566</v>
+        <v>-0.82103445162594202</v>
       </c>
       <c r="H101">
-        <v>-13.188151681546723</v>
+        <v>-9.2787985066105332</v>
       </c>
       <c r="I101">
-        <v>-0.82103445162594202</v>
+        <v>-11.496682400778614</v>
       </c>
       <c r="J101" s="8" t="s">
         <v>5</v>
@@ -3301,19 +3301,19 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C102">
-        <v>12.9</v>
+        <v>22.1</v>
       </c>
       <c r="E102">
-        <v>0.80479195817132831</v>
+        <v>0.79953276921025251</v>
       </c>
       <c r="G102">
-        <v>-11.78450269096427</v>
+        <v>-3.667403572553432</v>
       </c>
       <c r="H102">
-        <v>-13.550524736799877</v>
+        <v>-10.254685820424021</v>
       </c>
       <c r="I102">
-        <v>-4.2379750600333139</v>
+        <v>-14.458569083341761</v>
       </c>
       <c r="J102" s="8" t="s">
         <v>5</v>
@@ -3327,19 +3327,19 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C103">
-        <v>19.850000000000001</v>
+        <v>22</v>
       </c>
       <c r="E103">
-        <v>0.95948062545598045</v>
+        <v>0.96301360612015352</v>
       </c>
       <c r="G103">
-        <v>-17.219609480588574</v>
+        <v>-2.216119023979255</v>
       </c>
       <c r="H103">
-        <v>-16.707547416943914</v>
+        <v>-15.333531537197098</v>
       </c>
       <c r="I103">
-        <v>-1.7778680796496877</v>
+        <v>-19.875370284564013</v>
       </c>
       <c r="J103" s="8" t="s">
         <v>5</v>
@@ -3353,19 +3353,19 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C104">
-        <v>16.3</v>
+        <v>21.7</v>
       </c>
       <c r="E104">
-        <v>0.88084721194554993</v>
+        <v>0.88480140893325487</v>
       </c>
       <c r="G104">
-        <v>-7.7564409908445588</v>
+        <v>0.64076243664405053</v>
       </c>
       <c r="H104">
-        <v>-7.9694881967882036</v>
+        <v>-5.9644489338184563</v>
       </c>
       <c r="I104">
-        <v>0.64076243664405053</v>
+        <v>-10.09997713229156</v>
       </c>
       <c r="J104" s="8" t="s">
         <v>5</v>
@@ -3379,19 +3379,19 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C105">
-        <v>15.9</v>
+        <v>21.85</v>
       </c>
       <c r="E105">
-        <v>0.91315814381470517</v>
+        <v>0.89663324606822925</v>
       </c>
       <c r="G105">
-        <v>-6.9413046728587835</v>
+        <v>0.52049738092907083</v>
       </c>
       <c r="H105">
-        <v>-5.1769567826495875</v>
+        <v>-7.0028612879787744</v>
       </c>
       <c r="I105">
-        <v>1.2664879060061496</v>
+        <v>-7.2311374993775708</v>
       </c>
       <c r="J105" s="8" t="s">
         <v>5</v>
@@ -3405,19 +3405,19 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C106">
-        <v>18.45</v>
+        <v>17</v>
       </c>
       <c r="E106">
-        <v>0.94008303766094115</v>
+        <v>0.93018713388209662</v>
       </c>
       <c r="G106">
-        <v>-6.9677440379343265</v>
+        <v>-0.60993050070223354</v>
       </c>
       <c r="H106">
-        <v>-5.2362821846973651</v>
+        <v>-4.9215307292916117</v>
       </c>
       <c r="I106">
-        <v>-0.64182502893228099</v>
+        <v>-5.3924664867143823</v>
       </c>
       <c r="J106" s="8" t="s">
         <v>5</v>
@@ -3431,19 +3431,19 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C107">
-        <v>13.4</v>
+        <v>13</v>
       </c>
       <c r="E107">
-        <v>0.87072723425984577</v>
+        <v>0.87361151455216046</v>
       </c>
       <c r="G107">
-        <v>-13.957964348350156</v>
+        <v>-3.7781058098470046</v>
       </c>
       <c r="H107">
-        <v>-20.027867334749651</v>
+        <v>-9.3487525147202266</v>
       </c>
       <c r="I107">
-        <v>-3.7781058098470046</v>
+        <v>-16.232631183175652</v>
       </c>
       <c r="J107" s="8" t="s">
         <v>5</v>
@@ -3457,19 +3457,19 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C108">
-        <v>13.9</v>
+        <v>13</v>
       </c>
       <c r="E108">
-        <v>0.83022624907608422</v>
+        <v>0.84316709650591726</v>
       </c>
       <c r="G108">
-        <v>-7.0653485925206585</v>
+        <v>-1.1402013799636304</v>
       </c>
       <c r="H108">
-        <v>-9.6969648978278222</v>
+        <v>-5.571606990827215</v>
       </c>
       <c r="I108">
-        <v>-0.77311766667335557</v>
+        <v>-7.8784026836838317</v>
       </c>
       <c r="J108" s="8" t="s">
         <v>5</v>
@@ -3483,19 +3483,19 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C109">
-        <v>13.8</v>
+        <v>21.95</v>
       </c>
       <c r="E109">
-        <v>0.85384173337327618</v>
+        <v>0.85363158637315362</v>
       </c>
       <c r="G109">
-        <v>-6.6353794775643955</v>
+        <v>-1.7414844674323458</v>
       </c>
       <c r="H109">
-        <v>-6.6499319962508432</v>
+        <v>-6.9867616297320536</v>
       </c>
       <c r="I109">
-        <v>-1.7906776590122551</v>
+        <v>-5.1190252416242581</v>
       </c>
       <c r="J109" s="8" t="s">
         <v>5</v>
@@ -3509,19 +3509,19 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C110">
-        <v>15.8</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="E110">
-        <v>0.89807053728233166</v>
+        <v>0.89505330184715448</v>
       </c>
       <c r="G110">
-        <v>-12.070458765841401</v>
+        <v>-2.0836761129408869</v>
       </c>
       <c r="H110">
-        <v>-9.1302090002173415</v>
+        <v>-8.6290656194214517</v>
       </c>
       <c r="I110">
-        <v>-2.0836761129408869</v>
+        <v>-14.139133505947092</v>
       </c>
       <c r="J110" s="8" t="s">
         <v>5</v>
@@ -3535,19 +3535,19 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C111">
-        <v>16.8</v>
+        <v>12.9</v>
       </c>
       <c r="E111">
-        <v>0.9243788666712458</v>
+        <v>0.82324711381396676</v>
       </c>
       <c r="G111">
-        <v>-10.485621846606863</v>
+        <v>-4.9631874243965681</v>
       </c>
       <c r="H111">
-        <v>-15.482817157437504</v>
+        <v>-11.322733689273649</v>
       </c>
       <c r="I111">
-        <v>-4.3916972372085512</v>
+        <v>-11.261538624213289</v>
       </c>
       <c r="J111" s="8" t="s">
         <v>5</v>
@@ -3561,19 +3561,19 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C112">
-        <v>16.7</v>
+        <v>22.8</v>
       </c>
       <c r="E112">
-        <v>0.83183114324142793</v>
+        <v>0.91571864860762064</v>
       </c>
       <c r="G112">
-        <v>-12.889590553677898</v>
+        <v>-1.0421253697858033</v>
       </c>
       <c r="H112">
-        <v>-9.5916049385530009</v>
+        <v>-10.738114394349342</v>
       </c>
       <c r="I112">
-        <v>-1.0421253697858033</v>
+        <v>-15.545091425102747</v>
       </c>
       <c r="J112" s="8" t="s">
         <v>5</v>
@@ -3587,19 +3587,19 @@
     </row>
     <row r="113" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C113">
-        <v>19.7</v>
+        <v>13</v>
       </c>
       <c r="E113">
-        <v>0.97995340627636829</v>
+        <v>0.98380299182542985</v>
       </c>
       <c r="G113">
-        <v>-11.742031052016422</v>
+        <v>-1.7268333496518271</v>
       </c>
       <c r="H113">
-        <v>-12.089353963730792</v>
+        <v>-11.530235891581659</v>
       </c>
       <c r="I113">
-        <v>-1.7268333496518271</v>
+        <v>-11.64240335053324</v>
       </c>
       <c r="J113" s="8" t="s">
         <v>5</v>
@@ -3613,19 +3613,19 @@
     </row>
     <row r="114" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C114">
-        <v>16.899999999999999</v>
+        <v>22.25</v>
       </c>
       <c r="E114">
-        <v>0.8530639002438698</v>
+        <v>0.83717352329688455</v>
       </c>
       <c r="G114">
-        <v>-6.4506647631509377</v>
+        <v>-0.40621082032118927</v>
       </c>
       <c r="H114">
-        <v>-3.9658665246233284</v>
+        <v>-3.9223405847447212</v>
       </c>
       <c r="I114">
-        <v>-0.40621082032118927</v>
+        <v>-9.2831574220861111</v>
       </c>
       <c r="J114" s="8" t="s">
         <v>5</v>
@@ -3639,19 +3639,19 @@
     </row>
     <row r="115" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C115">
-        <v>16.350000000000001</v>
+        <v>14.55</v>
       </c>
       <c r="E115">
-        <v>0.95981837090327615</v>
+        <v>0.96167241132729331</v>
       </c>
       <c r="G115">
-        <v>-13.579184438492824</v>
+        <v>-3.1811509266898401</v>
       </c>
       <c r="H115">
-        <v>-15.083475031450908</v>
+        <v>-11.625168306944667</v>
       </c>
       <c r="I115">
-        <v>-3.1811509266898401</v>
+        <v>-14.767313307458037</v>
       </c>
       <c r="J115" s="8" t="s">
         <v>5</v>
@@ -3665,19 +3665,19 @@
     </row>
     <row r="116" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C116">
-        <v>18.600000000000001</v>
+        <v>14.5</v>
       </c>
       <c r="E116">
-        <v>0.96323078339371926</v>
+        <v>0.88758110003213231</v>
       </c>
       <c r="G116">
-        <v>-2.9949547232282754</v>
+        <v>-0.45167342564800905</v>
       </c>
       <c r="H116">
-        <v>-4.627363444757254</v>
+        <v>-2.9529689237100025</v>
       </c>
       <c r="I116">
-        <v>-0.48848928426671229</v>
+        <v>-5.0992555436013696</v>
       </c>
       <c r="J116" s="9" t="s">
         <v>3</v>
@@ -3690,17 +3690,20 @@
       </c>
     </row>
     <row r="117" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C117">
+        <v>18.3</v>
+      </c>
       <c r="E117">
-        <v>0.83810639034945722</v>
+        <v>0.95765638028691802</v>
       </c>
       <c r="G117">
-        <v>-6.4022711178918597</v>
+        <v>-1.3127041603990106</v>
       </c>
       <c r="H117">
-        <v>-8.826924437690236</v>
+        <v>-5.9710869340216819</v>
       </c>
       <c r="I117">
-        <v>-1.4913681998317136</v>
+        <v>-8.7067340888019782</v>
       </c>
       <c r="J117" s="9" t="s">
         <v>3</v>
@@ -3714,19 +3717,19 @@
     </row>
     <row r="118" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C118">
-        <v>18.55</v>
+        <v>13.850000000000001</v>
       </c>
       <c r="E118">
-        <v>0.95678221463793389</v>
+        <v>0.94037048914707277</v>
       </c>
       <c r="G118">
-        <v>-3.503903962034685</v>
+        <v>-1.1302880893423599</v>
       </c>
       <c r="H118">
-        <v>-4.4276711647987286</v>
+        <v>-4.1629464861200347</v>
       </c>
       <c r="I118">
-        <v>-1.2469614736468211</v>
+        <v>-4.7603572728166998</v>
       </c>
       <c r="J118" s="9" t="s">
         <v>3</v>
@@ -3743,16 +3746,16 @@
         <v>13</v>
       </c>
       <c r="E119">
-        <v>0.84124382737841108</v>
+        <v>0.87747833044915202</v>
       </c>
       <c r="G119">
-        <v>-5.752451693988581</v>
+        <v>-2.651294186354185</v>
       </c>
       <c r="H119">
-        <v>-5.8509549079533416</v>
+        <v>-5.7460518944664063</v>
       </c>
       <c r="I119">
-        <v>-2.651294186354185</v>
+        <v>-6.2759242848968793</v>
       </c>
       <c r="J119" s="9" t="s">
         <v>3</v>
@@ -3766,19 +3769,19 @@
     </row>
     <row r="120" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C120">
-        <v>14.95</v>
+        <v>15.9</v>
       </c>
       <c r="E120">
-        <v>0.93876137803225468</v>
+        <v>0.92733849483632258</v>
       </c>
       <c r="G120">
-        <v>-2.6763279094533088</v>
+        <v>-0.34902691820260928</v>
       </c>
       <c r="H120">
-        <v>-3.8867833680387052</v>
+        <v>-2.4899205704462557</v>
       </c>
       <c r="I120">
-        <v>-0.39340154947490585</v>
+        <v>-4.4376638119976546</v>
       </c>
       <c r="J120" s="9" t="s">
         <v>3</v>
@@ -3792,19 +3795,19 @@
     </row>
     <row r="121" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C121">
-        <v>19.8</v>
+        <v>17.95</v>
       </c>
       <c r="E121">
-        <v>0.92808431816075709</v>
+        <v>0.93593809910564763</v>
       </c>
       <c r="G121">
-        <v>-4.0884788792026505</v>
+        <v>2.2700124763534755E-2</v>
       </c>
       <c r="H121">
-        <v>-5.4099029138872812</v>
+        <v>-3.4718145076154179</v>
       </c>
       <c r="I121">
-        <v>2.2700124763534755E-2</v>
+        <v>-5.7480172365163478</v>
       </c>
       <c r="J121" s="9" t="s">
         <v>3</v>
@@ -3817,17 +3820,20 @@
       </c>
     </row>
     <row r="122" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <v>21.95</v>
+      </c>
       <c r="E122">
-        <v>0.80880108153687469</v>
+        <v>0.83308157749261436</v>
       </c>
       <c r="G122">
-        <v>-3.8064325110472201</v>
+        <v>-0.92726725253875986</v>
       </c>
       <c r="H122">
-        <v>-5.2187428351498912</v>
+        <v>-2.4881660759596933</v>
       </c>
       <c r="I122">
-        <v>-0.92726725253875986</v>
+        <v>-5.2901881248982043</v>
       </c>
       <c r="J122" s="9" t="s">
         <v>3</v>
@@ -3841,19 +3847,19 @@
     </row>
     <row r="123" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C123">
-        <v>14.7</v>
+        <v>16.3</v>
       </c>
       <c r="E123">
-        <v>0.91977497136293995</v>
+        <v>0.95565278465066106</v>
       </c>
       <c r="G123">
-        <v>-4.0746198794248194</v>
+        <v>-0.61767698810438298</v>
       </c>
       <c r="H123">
-        <v>-4.4384726415369871</v>
+        <v>-3.7319141229951578</v>
       </c>
       <c r="I123">
-        <v>-0.61767698810438298</v>
+        <v>-4.7457805558256361</v>
       </c>
       <c r="J123" s="9" t="s">
         <v>3</v>
@@ -3867,19 +3873,19 @@
     </row>
     <row r="124" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C124">
-        <v>17.3</v>
+        <v>15.05</v>
       </c>
       <c r="E124">
-        <v>0.95870184297651462</v>
+        <v>0.90874003351028332</v>
       </c>
       <c r="G124">
-        <v>-2.8511274512017573</v>
+        <v>-1.1106422034685179</v>
       </c>
       <c r="H124">
-        <v>-3.3587644541311823</v>
+        <v>-2.4306519128583082</v>
       </c>
       <c r="I124">
-        <v>-1.0897720503616746</v>
+        <v>-2.9178524704422135</v>
       </c>
       <c r="J124" s="9" t="s">
         <v>3</v>
@@ -3893,19 +3899,19 @@
     </row>
     <row r="125" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C125">
-        <v>14.7</v>
+        <v>13</v>
       </c>
       <c r="E125">
-        <v>0.89609873982442445</v>
+        <v>0.96363997601367846</v>
       </c>
       <c r="G125">
-        <v>-4.3370694631907059</v>
+        <v>-0.38069369676700354</v>
       </c>
       <c r="H125">
-        <v>-4.5873245093764305</v>
+        <v>-4.0881988820168829</v>
       </c>
       <c r="I125">
-        <v>-0.38069369676700354</v>
+        <v>-5.5780663826707624</v>
       </c>
       <c r="J125" s="9" t="s">
         <v>3</v>
@@ -3919,19 +3925,19 @@
     </row>
     <row r="126" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C126">
-        <v>16.5</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="E126">
-        <v>0.94815038828843456</v>
+        <v>0.94957770272281061</v>
       </c>
       <c r="G126">
-        <v>-3.9935722543414913</v>
+        <v>-0.7873190619669419</v>
       </c>
       <c r="H126">
-        <v>-5.2075433088331842</v>
+        <v>-2.7997821086014825</v>
       </c>
       <c r="I126">
-        <v>9.885405686320059E-2</v>
+        <v>-5.0888547229378265</v>
       </c>
       <c r="J126" s="9" t="s">
         <v>3</v>
@@ -3945,19 +3951,19 @@
     </row>
     <row r="127" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C127">
-        <v>19.3</v>
+        <v>13.3</v>
       </c>
       <c r="E127">
-        <v>0.98364470183906783</v>
+        <v>0.97877239176023978</v>
       </c>
       <c r="G127">
-        <v>-8.2883599328729716</v>
+        <v>-0.5074204469101713</v>
       </c>
       <c r="H127">
-        <v>-9.6572151752761108</v>
+        <v>-6.4548222100003123</v>
       </c>
       <c r="I127">
-        <v>-0.5074204469101713</v>
+        <v>-9.2810036224946444</v>
       </c>
       <c r="J127" s="9" t="s">
         <v>3</v>
@@ -3971,19 +3977,19 @@
     </row>
     <row r="128" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C128">
-        <v>19.95</v>
+        <v>13.5</v>
       </c>
       <c r="E128">
-        <v>0.98684609962405578</v>
+        <v>0.98150234432944516</v>
       </c>
       <c r="G128">
-        <v>-7.5886173369799756</v>
+        <v>-0.64744885376766914</v>
       </c>
       <c r="H128">
-        <v>-8.113123234331848</v>
+        <v>-6.0658077870602449</v>
       </c>
       <c r="I128">
-        <v>-0.55844788054102501</v>
+        <v>-8.5964359549806542</v>
       </c>
       <c r="J128" s="9" t="s">
         <v>3</v>
@@ -3997,19 +4003,19 @@
     </row>
     <row r="129" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C129">
-        <v>18.2</v>
+        <v>14.8</v>
       </c>
       <c r="E129">
-        <v>0.9591321451686794</v>
+        <v>0.94678056289661316</v>
       </c>
       <c r="G129">
-        <v>-4.9870102494330713</v>
+        <v>-1.003941455493879</v>
       </c>
       <c r="H129">
-        <v>-6.6829683735596186</v>
+        <v>-3.3723333824236117</v>
       </c>
       <c r="I129">
-        <v>-0.62278067715339047</v>
+        <v>-6.2613301682658271</v>
       </c>
       <c r="J129" s="9" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fixing missing value error in retime
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
+++ b/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B6C93C-258C-7342-84DA-EE6FF5432702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2062735-6C8F-E74D-81EA-189E795E621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
+    <workbookView xWindow="380" yWindow="7540" windowWidth="35840" windowHeight="21940" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Tstar" sheetId="1" r:id="rId1"/>
@@ -506,8 +506,8 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,7 +1151,7 @@
         <v>-0.94745318113980681</v>
       </c>
       <c r="F22">
-        <v>0.43326617188422362</v>
+        <v>0.38646480451653992</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>3</v>
@@ -1177,7 +1177,7 @@
         <v>-0.87429843791886563</v>
       </c>
       <c r="F23">
-        <v>0.27328101589573639</v>
+        <v>0.27527856208311324</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>3</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>15</v>
+        <v>15.75</v>
       </c>
       <c r="B24">
         <v>16.5</v>
@@ -1203,7 +1203,7 @@
         <v>-0.85406217608592705</v>
       </c>
       <c r="F24">
-        <v>0.22774839719706286</v>
+        <v>0.17456895282104468</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>3</v>
@@ -1229,7 +1229,7 @@
         <v>0.31582232251363646</v>
       </c>
       <c r="F25">
-        <v>0.57717258267476512</v>
+        <v>0.59934801604464083</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>3</v>
@@ -1255,7 +1255,7 @@
         <v>-0.85223374965078624</v>
       </c>
       <c r="F26">
-        <v>0.7906876067260824</v>
+        <v>0.75480289094797293</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>3</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>15</v>
+        <v>14.9</v>
       </c>
       <c r="B27">
         <v>18.5</v>
@@ -1281,7 +1281,7 @@
         <v>-0.81481619507567182</v>
       </c>
       <c r="F27">
-        <v>0.62516706958913748</v>
+        <v>0.47186482247471007</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>3</v>
@@ -1307,7 +1307,7 @@
         <v>-0.97117380928489072</v>
       </c>
       <c r="F28">
-        <v>0.60172111206937362</v>
+        <v>0.53679661222589958</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>3</v>
@@ -1333,7 +1333,7 @@
         <v>-0.69725428572718851</v>
       </c>
       <c r="F29">
-        <v>0.68418000644285704</v>
+        <v>0.65602492512713406</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>3</v>
@@ -1356,10 +1356,10 @@
         <v>13.7</v>
       </c>
       <c r="E30">
-        <v>-0.64747030794752858</v>
+        <v>-0.70068501135002781</v>
       </c>
       <c r="F30">
-        <v>0.16413913295754096</v>
+        <v>0.18579398848600134</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>3</v>
@@ -1385,7 +1385,7 @@
         <v>-0.9082180753885768</v>
       </c>
       <c r="F31">
-        <v>0.39543966305406886</v>
+        <v>0.30278033521933467</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>3</v>
@@ -1411,7 +1411,7 @@
         <v>-0.91300568958524009</v>
       </c>
       <c r="F32">
-        <v>0.48356198230444392</v>
+        <v>0.51513287442007083</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>3</v>
@@ -1437,7 +1437,7 @@
         <v>-0.77358162923952567</v>
       </c>
       <c r="F33">
-        <v>0.27359892530456126</v>
+        <v>7.8346526759103016E-2</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>3</v>
@@ -1463,7 +1463,7 @@
         <v>-0.96807122700840376</v>
       </c>
       <c r="F34">
-        <v>0.47264788299450933</v>
+        <v>0.45475000823733486</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>3</v>
@@ -1486,10 +1486,10 @@
         <v>13.6</v>
       </c>
       <c r="E35">
-        <v>-0.91290085207471461</v>
+        <v>-0.91297172016467165</v>
       </c>
       <c r="F35">
-        <v>0.25058528955179382</v>
+        <v>6.7500850207241794E-2</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>3</v>
@@ -1515,7 +1515,7 @@
         <v>-0.87399609135327805</v>
       </c>
       <c r="F36">
-        <v>0.46059491923894336</v>
+        <v>0.28271455563306036</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>3</v>
@@ -1541,7 +1541,7 @@
         <v>-0.70807857798906715</v>
       </c>
       <c r="F37">
-        <v>0.67549401025931455</v>
+        <v>0.57218212269925961</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Adding plot of temperatures in specific timebins for cooling stimulus
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
+++ b/Code/Plotting in R/Data/AFDResponse_R_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2062735-6C8F-E74D-81EA-189E795E621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B11A65F-C599-2C43-A7A8-C15A9ED8571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="7540" windowWidth="35840" windowHeight="21940" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{119B291C-68D2-2942-B3A2-5929EB731D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Tstar" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="20">
   <si>
     <t>Temperature</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Time_460s</t>
+  </si>
+  <si>
+    <t>Temp_220s</t>
+  </si>
+  <si>
+    <t>Temp_340s</t>
+  </si>
+  <si>
+    <t>Temp_460s</t>
   </si>
 </sst>
 </file>
@@ -503,11 +512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185A0AF1-AEF1-B74F-8EB8-314724BE975D}">
-  <dimension ref="A1:L130"/>
+  <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22:F37"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J116" sqref="J116:L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,7 +528,7 @@
     <col min="6" max="9" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -548,16 +557,25 @@
         <v>16</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>21.55</v>
       </c>
@@ -576,17 +594,17 @@
       <c r="F2">
         <v>0.87620656492906002</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>21.5</v>
       </c>
@@ -605,17 +623,17 @@
       <c r="F3">
         <v>0.86499828740207418</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>21.9</v>
       </c>
@@ -634,17 +652,17 @@
       <c r="F4">
         <v>0.75912487227141368</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>21.7</v>
       </c>
@@ -663,17 +681,17 @@
       <c r="F5">
         <v>0.81328907732604849</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>22.1</v>
       </c>
@@ -692,17 +710,17 @@
       <c r="F6">
         <v>0.76791897991468883</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>21.75</v>
       </c>
@@ -721,17 +739,17 @@
       <c r="F7">
         <v>0.82163833487408511</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21.7</v>
       </c>
@@ -750,17 +768,17 @@
       <c r="F8">
         <v>0.79025536751138226</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>22.3</v>
       </c>
@@ -779,17 +797,17 @@
       <c r="F9">
         <v>0.77393495229361153</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21.7</v>
       </c>
@@ -808,17 +826,17 @@
       <c r="F10">
         <v>0.90890363505798</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21.8</v>
       </c>
@@ -837,17 +855,17 @@
       <c r="F11">
         <v>0.84978018586947968</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22</v>
       </c>
@@ -866,17 +884,17 @@
       <c r="F12">
         <v>0.76053395616890618</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L12" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>22.25</v>
       </c>
@@ -895,17 +913,17 @@
       <c r="F13">
         <v>0.8485236101831124</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21.9</v>
       </c>
@@ -924,17 +942,17 @@
       <c r="F14">
         <v>0.81023401821957952</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>21.8</v>
       </c>
@@ -953,17 +971,17 @@
       <c r="F15">
         <v>0.84118035282600501</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>22.3</v>
       </c>
@@ -982,17 +1000,17 @@
       <c r="F16">
         <v>0.61025224355803498</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>22.7</v>
       </c>
@@ -1011,17 +1029,17 @@
       <c r="F17">
         <v>0.51052425674684365</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>21.9</v>
       </c>
@@ -1040,17 +1058,17 @@
       <c r="F18">
         <v>0.7732192450349501</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L18" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>21.7</v>
       </c>
@@ -1069,17 +1087,17 @@
       <c r="F19">
         <v>0.72160562832309039</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>22.15</v>
       </c>
@@ -1098,17 +1116,17 @@
       <c r="F20">
         <v>0.6660345400084875</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L20" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>22.3</v>
       </c>
@@ -1127,17 +1145,17 @@
       <c r="F21">
         <v>0.64786216508986871</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>15.95</v>
       </c>
@@ -1153,17 +1171,17 @@
       <c r="F22">
         <v>0.38646480451653992</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>15.8</v>
       </c>
@@ -1179,17 +1197,17 @@
       <c r="F23">
         <v>0.27527856208311324</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L23" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15.75</v>
       </c>
@@ -1205,17 +1223,17 @@
       <c r="F24">
         <v>0.17456895282104468</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O24" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>15.45</v>
       </c>
@@ -1231,17 +1249,17 @@
       <c r="F25">
         <v>0.59934801604464083</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O25" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>14.2</v>
       </c>
@@ -1257,17 +1275,17 @@
       <c r="F26">
         <v>0.75480289094797293</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>14.9</v>
       </c>
@@ -1283,17 +1301,17 @@
       <c r="F27">
         <v>0.47186482247471007</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O27" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>15.4</v>
       </c>
@@ -1309,17 +1327,17 @@
       <c r="F28">
         <v>0.53679661222589958</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>15</v>
       </c>
@@ -1335,17 +1353,17 @@
       <c r="F29">
         <v>0.65602492512713406</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>16.149999999999999</v>
       </c>
@@ -1361,17 +1379,17 @@
       <c r="F30">
         <v>0.18579398848600134</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L30" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15.1</v>
       </c>
@@ -1387,17 +1405,17 @@
       <c r="F31">
         <v>0.30278033521933467</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L31" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O31" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>15.8</v>
       </c>
@@ -1413,17 +1431,17 @@
       <c r="F32">
         <v>0.51513287442007083</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L32" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>14.6</v>
       </c>
@@ -1439,17 +1457,17 @@
       <c r="F33">
         <v>7.8346526759103016E-2</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L33" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O33" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14.6</v>
       </c>
@@ -1465,17 +1483,17 @@
       <c r="F34">
         <v>0.45475000823733486</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L34" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O34" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>15.2</v>
       </c>
@@ -1491,17 +1509,17 @@
       <c r="F35">
         <v>6.7500850207241794E-2</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L35" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>15.1</v>
       </c>
@@ -1517,17 +1535,17 @@
       <c r="F36">
         <v>0.28271455563306036</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L36" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>14.3</v>
       </c>
@@ -1543,17 +1561,17 @@
       <c r="F37">
         <v>0.57218212269925961</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L37" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>16.399999999999999</v>
       </c>
@@ -1569,17 +1587,17 @@
       <c r="F38">
         <v>-0.35468711415254744</v>
       </c>
-      <c r="J38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K38" s="3" t="s">
+      <c r="M38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L38" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O38" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>14.6</v>
       </c>
@@ -1595,17 +1613,17 @@
       <c r="F39">
         <v>0.78321233428325499</v>
       </c>
-      <c r="J39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K39" s="3" t="s">
+      <c r="M39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L39" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O39" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>16.100000000000001</v>
       </c>
@@ -1621,17 +1639,17 @@
       <c r="F40">
         <v>-0.28418983671617015</v>
       </c>
-      <c r="J40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K40" s="3" t="s">
+      <c r="M40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L40" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O40" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>16.600000000000001</v>
       </c>
@@ -1647,17 +1665,17 @@
       <c r="F41">
         <v>0.13815113759883346</v>
       </c>
-      <c r="J41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K41" s="3" t="s">
+      <c r="M41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L41" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O41" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>16.600000000000001</v>
       </c>
@@ -1673,17 +1691,17 @@
       <c r="F42">
         <v>-0.37012283450094674</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K42" s="3" t="s">
+      <c r="M42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L42" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O42" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16.8</v>
       </c>
@@ -1699,17 +1717,17 @@
       <c r="F43">
         <v>4.1254882511444221E-4</v>
       </c>
-      <c r="J43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K43" s="3" t="s">
+      <c r="M43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L43" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O43" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17.2</v>
       </c>
@@ -1725,17 +1743,17 @@
       <c r="F44">
         <v>4.9675196276855613E-2</v>
       </c>
-      <c r="J44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K44" s="3" t="s">
+      <c r="M44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N44" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O44" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>17.166666666666668</v>
       </c>
@@ -1751,17 +1769,17 @@
       <c r="F45">
         <v>0.23756288947089624</v>
       </c>
-      <c r="J45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K45" s="3" t="s">
+      <c r="M45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L45" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O45" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>16.899999999999999</v>
       </c>
@@ -1777,17 +1795,17 @@
       <c r="F46">
         <v>-1.9206502532388266E-2</v>
       </c>
-      <c r="J46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K46" s="3" t="s">
+      <c r="M46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N46" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L46" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O46" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>15.4</v>
       </c>
@@ -1803,17 +1821,17 @@
       <c r="F47">
         <v>0.63612748233707095</v>
       </c>
-      <c r="J47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K47" s="3" t="s">
+      <c r="M47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L47" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O47" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>15.55</v>
       </c>
@@ -1829,17 +1847,17 @@
       <c r="F48">
         <v>0.45356309520275401</v>
       </c>
-      <c r="J48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K48" s="3" t="s">
+      <c r="M48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L48" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O48" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>17.55</v>
       </c>
@@ -1855,17 +1873,17 @@
       <c r="F49">
         <v>-0.21711472081928962</v>
       </c>
-      <c r="J49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K49" s="3" t="s">
+      <c r="M49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L49" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O49" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>15</v>
       </c>
@@ -1881,17 +1899,17 @@
       <c r="F50">
         <v>0.65584092685818418</v>
       </c>
-      <c r="J50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K50" s="3" t="s">
+      <c r="M50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L50" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O50" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>17.45</v>
       </c>
@@ -1907,17 +1925,17 @@
       <c r="F51">
         <v>-7.4318967839932864E-3</v>
       </c>
-      <c r="J51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K51" s="3" t="s">
+      <c r="M51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L51" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O51" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>16.100000000000001</v>
       </c>
@@ -1933,17 +1951,17 @@
       <c r="F52">
         <v>0.37996868279131446</v>
       </c>
-      <c r="J52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K52" s="3" t="s">
+      <c r="M52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L52" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O52" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>17.399999999999999</v>
       </c>
@@ -1959,17 +1977,17 @@
       <c r="F53">
         <v>-2.7443505841859136E-3</v>
       </c>
-      <c r="J53" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K53" s="3" t="s">
+      <c r="M53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N53" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L53" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O53" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>17.95</v>
       </c>
@@ -1985,17 +2003,17 @@
       <c r="F54">
         <v>9.3604945564630879E-2</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L54" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O54" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>17.2</v>
       </c>
@@ -2011,17 +2029,17 @@
       <c r="F55">
         <v>-0.17235037784049473</v>
       </c>
-      <c r="J55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L55" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N55" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O55" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>14.2</v>
       </c>
@@ -2037,17 +2055,17 @@
       <c r="F56">
         <v>0.85814681276978866</v>
       </c>
-      <c r="J56" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L56" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O56" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>17.2</v>
       </c>
@@ -2063,17 +2081,17 @@
       <c r="F57">
         <v>0.10035758344004961</v>
       </c>
-      <c r="J57" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L57" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>16.5</v>
       </c>
@@ -2089,17 +2107,17 @@
       <c r="F58">
         <v>0.13530719911392941</v>
       </c>
-      <c r="J58" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L58" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O58" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>13.9</v>
       </c>
@@ -2115,17 +2133,17 @@
       <c r="F59">
         <v>-5.6628875371643746E-2</v>
       </c>
-      <c r="J59" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L59" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O59" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>16.100000000000001</v>
       </c>
@@ -2141,17 +2159,17 @@
       <c r="F60">
         <v>1.6409415015681147E-2</v>
       </c>
-      <c r="J60" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L60" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>16.8</v>
       </c>
@@ -2167,17 +2185,17 @@
       <c r="F61">
         <v>0.36445026465509434</v>
       </c>
-      <c r="J61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L61" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O61" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>15.9</v>
       </c>
@@ -2193,17 +2211,17 @@
       <c r="F62">
         <v>-0.3266055982325563</v>
       </c>
-      <c r="J62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L62" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O62" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>15.4</v>
       </c>
@@ -2219,17 +2237,17 @@
       <c r="F63">
         <v>5.602332462341756E-2</v>
       </c>
-      <c r="J63" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L63" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O63" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>16.899999999999999</v>
       </c>
@@ -2245,17 +2263,17 @@
       <c r="F64">
         <v>-5.3019985672463139E-2</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L64" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O64" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>16.600000000000001</v>
       </c>
@@ -2271,17 +2289,17 @@
       <c r="F65">
         <v>-0.29803192820808327</v>
       </c>
-      <c r="J65" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L65" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O65" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>17.3</v>
       </c>
@@ -2297,17 +2315,17 @@
       <c r="F66">
         <v>0.50314569878788085</v>
       </c>
-      <c r="J66" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L66" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O66" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>16.3</v>
       </c>
@@ -2323,17 +2341,17 @@
       <c r="F67">
         <v>-7.8354101056984579E-2</v>
       </c>
-      <c r="J67" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L67" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O67" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>17.600000000000001</v>
       </c>
@@ -2349,17 +2367,17 @@
       <c r="F68">
         <v>0.31356448905668372</v>
       </c>
-      <c r="J68" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L68" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O68" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>17.2</v>
       </c>
@@ -2375,17 +2393,17 @@
       <c r="F69">
         <v>0.26373679623384222</v>
       </c>
-      <c r="J69" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K69" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L69" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O69" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>14.9</v>
       </c>
@@ -2401,17 +2419,17 @@
       <c r="F70">
         <v>0.67545967490877601</v>
       </c>
-      <c r="J70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L70" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O70" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>21.7</v>
       </c>
@@ -2430,17 +2448,17 @@
       <c r="F71">
         <v>-0.66445754496138287</v>
       </c>
-      <c r="J71" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L71" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N71" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O71" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>21.8</v>
       </c>
@@ -2459,17 +2477,17 @@
       <c r="F72">
         <v>-0.53254796212427669</v>
       </c>
-      <c r="J72" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K72" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L72" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N72" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O72" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>22.15</v>
       </c>
@@ -2488,17 +2506,17 @@
       <c r="F73">
         <v>-0.7036309670169929</v>
       </c>
-      <c r="J73" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K73" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L73" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O73" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>22.5</v>
       </c>
@@ -2517,17 +2535,17 @@
       <c r="F74">
         <v>-0.43567608455688417</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K74" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L74" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O74" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>21.25</v>
       </c>
@@ -2546,17 +2564,17 @@
       <c r="F75">
         <v>0.68489449660582447</v>
       </c>
-      <c r="J75" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L75" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O75" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>20.8</v>
       </c>
@@ -2575,17 +2593,17 @@
       <c r="F76">
         <v>-0.5485967995740485</v>
       </c>
-      <c r="J76" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L76" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O76" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>21.4</v>
       </c>
@@ -2604,17 +2622,17 @@
       <c r="F77">
         <v>-0.66685620290276915</v>
       </c>
-      <c r="J77" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L77" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O77" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>21.2</v>
       </c>
@@ -2633,17 +2651,17 @@
       <c r="F78">
         <v>-0.73321349043009776</v>
       </c>
-      <c r="J78" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K78" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L78" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M78" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O78" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>20.6</v>
       </c>
@@ -2662,17 +2680,17 @@
       <c r="F79">
         <v>-0.4317445392996942</v>
       </c>
-      <c r="J79" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K79" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L79" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M79" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N79" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O79" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>21.1</v>
       </c>
@@ -2691,17 +2709,17 @@
       <c r="F80">
         <v>0.67460743658293876</v>
       </c>
-      <c r="J80" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L80" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O80" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>20.95</v>
       </c>
@@ -2720,17 +2738,17 @@
       <c r="F81">
         <v>-0.64979773843335986</v>
       </c>
-      <c r="J81" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K81" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L81" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O81" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>21.4</v>
       </c>
@@ -2749,17 +2767,17 @@
       <c r="F82">
         <v>0.49675849262517019</v>
       </c>
-      <c r="J82" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K82" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L82" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M82" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N82" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O82" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>21.8</v>
       </c>
@@ -2778,17 +2796,17 @@
       <c r="F83">
         <v>-0.62926104357193302</v>
       </c>
-      <c r="J83" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K83" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L83" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M83" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O83" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>21</v>
       </c>
@@ -2807,17 +2825,17 @@
       <c r="F84">
         <v>-0.64320095905743668</v>
       </c>
-      <c r="J84" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L84" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O84" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>21.6</v>
       </c>
@@ -2836,17 +2854,17 @@
       <c r="F85">
         <v>-0.66751999097012149</v>
       </c>
-      <c r="J85" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K85" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L85" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N85" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O85" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>30.8</v>
       </c>
@@ -2865,17 +2883,17 @@
       <c r="F86">
         <v>-0.19987674817500992</v>
       </c>
-      <c r="J86" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K86" s="6" t="s">
+      <c r="M86" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N86" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L86" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O86" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>20.95</v>
       </c>
@@ -2894,17 +2912,17 @@
       <c r="F87">
         <v>-0.59212413665189545</v>
       </c>
-      <c r="J87" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K87" s="6" t="s">
+      <c r="M87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N87" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L87" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O87" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>21.900000000000002</v>
       </c>
@@ -2923,17 +2941,17 @@
       <c r="F88">
         <v>-0.58784109198231105</v>
       </c>
-      <c r="J88" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K88" s="6" t="s">
+      <c r="M88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N88" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L88" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O88" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>21.7</v>
       </c>
@@ -2952,17 +2970,17 @@
       <c r="F89">
         <v>-0.5284133750374993</v>
       </c>
-      <c r="J89" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K89" s="6" t="s">
+      <c r="M89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N89" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L89" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O89" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>21</v>
       </c>
@@ -2981,17 +2999,17 @@
       <c r="F90">
         <v>-0.41177849391936738</v>
       </c>
-      <c r="J90" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K90" s="6" t="s">
+      <c r="M90" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N90" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L90" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O90" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>21.55</v>
       </c>
@@ -3010,17 +3028,17 @@
       <c r="F91">
         <v>-0.6306457048267563</v>
       </c>
-      <c r="J91" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K91" s="6" t="s">
+      <c r="M91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N91" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L91" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O91" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>21.6</v>
       </c>
@@ -3039,17 +3057,17 @@
       <c r="F92">
         <v>-0.62741417317434756</v>
       </c>
-      <c r="J92" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K92" s="6" t="s">
+      <c r="M92" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N92" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L92" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O92" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>20.9</v>
       </c>
@@ -3068,17 +3086,17 @@
       <c r="F93">
         <v>0.8331822964171659</v>
       </c>
-      <c r="J93" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K93" s="6" t="s">
+      <c r="M93" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N93" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L93" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O93" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>21.5</v>
       </c>
@@ -3097,17 +3115,17 @@
       <c r="F94">
         <v>-0.61533371803104908</v>
       </c>
-      <c r="J94" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K94" s="6" t="s">
+      <c r="M94" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N94" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L94" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O94" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>21.9</v>
       </c>
@@ -3126,17 +3144,17 @@
       <c r="F95">
         <v>-0.68401204240061619</v>
       </c>
-      <c r="J95" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K95" s="6" t="s">
+      <c r="M95" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N95" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L95" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O95" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>21.7</v>
       </c>
@@ -3155,17 +3173,17 @@
       <c r="F96">
         <v>-0.63791946495868002</v>
       </c>
-      <c r="J96" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K96" s="6" t="s">
+      <c r="M96" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N96" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L96" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O96" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>24.4</v>
       </c>
@@ -3184,17 +3202,17 @@
       <c r="F97">
         <v>0.79750440794363198</v>
       </c>
-      <c r="J97" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K97" s="6" t="s">
+      <c r="M97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N97" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L97" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O97" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>20.9</v>
       </c>
@@ -3213,17 +3231,17 @@
       <c r="F98">
         <v>-0.56989275755158186</v>
       </c>
-      <c r="J98" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K98" s="6" t="s">
+      <c r="M98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N98" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L98" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O98" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>22</v>
       </c>
@@ -3242,17 +3260,17 @@
       <c r="F99">
         <v>-0.64049339111595094</v>
       </c>
-      <c r="J99" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K99" s="6" t="s">
+      <c r="M99" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N99" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L99" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O99" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>21.6</v>
       </c>
@@ -3271,17 +3289,17 @@
       <c r="F100">
         <v>-0.62447644261218405</v>
       </c>
-      <c r="J100" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K100" s="6" t="s">
+      <c r="M100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N100" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L100" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O100" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C101">
         <v>22.35</v>
       </c>
@@ -3297,17 +3315,26 @@
       <c r="I101">
         <v>-11.496682400778614</v>
       </c>
-      <c r="J101" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K101" s="8" t="s">
+      <c r="J101">
+        <v>21.9</v>
+      </c>
+      <c r="K101">
+        <v>13.6</v>
+      </c>
+      <c r="L101">
+        <v>13</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N101" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L101" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O101" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C102">
         <v>22.1</v>
       </c>
@@ -3323,17 +3350,26 @@
       <c r="I102">
         <v>-14.458569083341761</v>
       </c>
-      <c r="J102" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K102" s="8" t="s">
+      <c r="J102">
+        <v>22</v>
+      </c>
+      <c r="K102">
+        <v>13.55</v>
+      </c>
+      <c r="L102">
+        <v>13</v>
+      </c>
+      <c r="M102" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N102" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L102" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O102" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C103">
         <v>22</v>
       </c>
@@ -3349,17 +3385,26 @@
       <c r="I103">
         <v>-19.875370284564013</v>
       </c>
-      <c r="J103" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K103" s="8" t="s">
+      <c r="J103">
+        <v>21.900000000000002</v>
+      </c>
+      <c r="K103">
+        <v>13.700000000000001</v>
+      </c>
+      <c r="L103">
+        <v>13</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N103" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L103" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O103" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C104">
         <v>21.7</v>
       </c>
@@ -3375,17 +3420,26 @@
       <c r="I104">
         <v>-10.09997713229156</v>
       </c>
-      <c r="J104" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K104" s="8" t="s">
+      <c r="J104">
+        <v>22</v>
+      </c>
+      <c r="K104">
+        <v>13.8</v>
+      </c>
+      <c r="L104">
+        <v>13</v>
+      </c>
+      <c r="M104" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N104" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L104" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O104" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C105">
         <v>21.85</v>
       </c>
@@ -3401,17 +3455,26 @@
       <c r="I105">
         <v>-7.2311374993775708</v>
       </c>
-      <c r="J105" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K105" s="8" t="s">
+      <c r="J105">
+        <v>21.95</v>
+      </c>
+      <c r="K105">
+        <v>13.6</v>
+      </c>
+      <c r="L105">
+        <v>13</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N105" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L105" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O105" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C106">
         <v>17</v>
       </c>
@@ -3427,17 +3490,26 @@
       <c r="I106">
         <v>-5.3924664867143823</v>
       </c>
-      <c r="J106" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K106" s="8" t="s">
+      <c r="J106">
+        <v>21.95</v>
+      </c>
+      <c r="K106">
+        <v>13.8</v>
+      </c>
+      <c r="L106">
+        <v>13</v>
+      </c>
+      <c r="M106" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N106" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L106" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O106" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C107">
         <v>13</v>
       </c>
@@ -3453,17 +3525,26 @@
       <c r="I107">
         <v>-16.232631183175652</v>
       </c>
-      <c r="J107" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K107" s="8" t="s">
+      <c r="J107">
+        <v>22</v>
+      </c>
+      <c r="K107">
+        <v>13.9</v>
+      </c>
+      <c r="L107">
+        <v>13</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N107" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L107" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O107" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C108">
         <v>13</v>
       </c>
@@ -3479,17 +3560,26 @@
       <c r="I108">
         <v>-7.8784026836838317</v>
       </c>
-      <c r="J108" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K108" s="8" t="s">
+      <c r="J108">
+        <v>22</v>
+      </c>
+      <c r="K108">
+        <v>13.95</v>
+      </c>
+      <c r="L108">
+        <v>13</v>
+      </c>
+      <c r="M108" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N108" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L108" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O108" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C109">
         <v>21.95</v>
       </c>
@@ -3505,17 +3595,26 @@
       <c r="I109">
         <v>-5.1190252416242581</v>
       </c>
-      <c r="J109" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K109" s="8" t="s">
+      <c r="J109">
+        <v>22</v>
+      </c>
+      <c r="K109">
+        <v>13.7</v>
+      </c>
+      <c r="L109">
+        <v>13</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N109" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L109" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O109" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C110">
         <v>17.100000000000001</v>
       </c>
@@ -3531,17 +3630,26 @@
       <c r="I110">
         <v>-14.139133505947092</v>
       </c>
-      <c r="J110" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K110" s="8" t="s">
+      <c r="J110">
+        <v>22</v>
+      </c>
+      <c r="K110">
+        <v>13.8</v>
+      </c>
+      <c r="L110">
+        <v>13</v>
+      </c>
+      <c r="M110" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N110" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L110" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O110" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C111">
         <v>12.9</v>
       </c>
@@ -3557,17 +3665,26 @@
       <c r="I111">
         <v>-11.261538624213289</v>
       </c>
-      <c r="J111" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K111" s="8" t="s">
+      <c r="J111">
+        <v>21.9</v>
+      </c>
+      <c r="K111">
+        <v>13.7</v>
+      </c>
+      <c r="L111">
+        <v>12.9</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N111" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L111" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O111" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C112">
         <v>22.8</v>
       </c>
@@ -3583,17 +3700,26 @@
       <c r="I112">
         <v>-15.545091425102747</v>
       </c>
-      <c r="J112" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K112" s="8" t="s">
+      <c r="J112">
+        <v>22</v>
+      </c>
+      <c r="K112">
+        <v>13.3</v>
+      </c>
+      <c r="L112">
+        <v>13</v>
+      </c>
+      <c r="M112" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N112" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L112" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="113" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O112" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="113" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C113">
         <v>13</v>
       </c>
@@ -3609,17 +3735,26 @@
       <c r="I113">
         <v>-11.64240335053324</v>
       </c>
-      <c r="J113" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K113" s="8" t="s">
+      <c r="J113">
+        <v>21.9</v>
+      </c>
+      <c r="K113">
+        <v>13.4</v>
+      </c>
+      <c r="L113">
+        <v>12.9</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N113" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L113" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="114" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O113" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C114">
         <v>22.25</v>
       </c>
@@ -3635,17 +3770,26 @@
       <c r="I114">
         <v>-9.2831574220861111</v>
       </c>
-      <c r="J114" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K114" s="8" t="s">
+      <c r="J114">
+        <v>21.9</v>
+      </c>
+      <c r="K114">
+        <v>13.7</v>
+      </c>
+      <c r="L114">
+        <v>13</v>
+      </c>
+      <c r="M114" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N114" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L114" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="115" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O114" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C115">
         <v>14.55</v>
       </c>
@@ -3661,17 +3805,26 @@
       <c r="I115">
         <v>-14.767313307458037</v>
       </c>
-      <c r="J115" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K115" s="8" t="s">
+      <c r="J115">
+        <v>21.9</v>
+      </c>
+      <c r="K115">
+        <v>13.6</v>
+      </c>
+      <c r="L115">
+        <v>13</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N115" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L115" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="116" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O115" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C116">
         <v>14.5</v>
       </c>
@@ -3687,17 +3840,26 @@
       <c r="I116">
         <v>-5.0992555436013696</v>
       </c>
-      <c r="J116" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K116" s="9" t="s">
+      <c r="J116">
+        <v>22</v>
+      </c>
+      <c r="K116">
+        <v>13.2</v>
+      </c>
+      <c r="L116">
+        <v>12.9</v>
+      </c>
+      <c r="M116" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N116" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L116" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="117" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O116" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C117">
         <v>18.3</v>
       </c>
@@ -3713,17 +3875,26 @@
       <c r="I117">
         <v>-8.7067340888019782</v>
       </c>
-      <c r="J117" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K117" s="9" t="s">
+      <c r="J117">
+        <v>21.9</v>
+      </c>
+      <c r="K117">
+        <v>13.3</v>
+      </c>
+      <c r="L117">
+        <v>13</v>
+      </c>
+      <c r="M117" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N117" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L117" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="118" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O117" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C118">
         <v>13.850000000000001</v>
       </c>
@@ -3739,17 +3910,26 @@
       <c r="I118">
         <v>-4.7603572728166998</v>
       </c>
-      <c r="J118" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K118" s="9" t="s">
+      <c r="J118">
+        <v>22.1</v>
+      </c>
+      <c r="K118">
+        <v>13.5</v>
+      </c>
+      <c r="L118">
+        <v>13</v>
+      </c>
+      <c r="M118" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N118" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L118" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="119" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O118" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C119">
         <v>13</v>
       </c>
@@ -3765,17 +3945,26 @@
       <c r="I119">
         <v>-6.2759242848968793</v>
       </c>
-      <c r="J119" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K119" s="9" t="s">
+      <c r="J119">
+        <v>21.95</v>
+      </c>
+      <c r="K119">
+        <v>13.5</v>
+      </c>
+      <c r="L119">
+        <v>13</v>
+      </c>
+      <c r="M119" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N119" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L119" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="120" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O119" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C120">
         <v>15.9</v>
       </c>
@@ -3791,17 +3980,26 @@
       <c r="I120">
         <v>-4.4376638119976546</v>
       </c>
-      <c r="J120" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K120" s="9" t="s">
+      <c r="J120">
+        <v>21.9</v>
+      </c>
+      <c r="K120">
+        <v>13.3</v>
+      </c>
+      <c r="L120">
+        <v>13</v>
+      </c>
+      <c r="M120" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N120" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L120" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="121" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O120" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C121">
         <v>17.95</v>
       </c>
@@ -3817,17 +4015,26 @@
       <c r="I121">
         <v>-5.7480172365163478</v>
       </c>
-      <c r="J121" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K121" s="9" t="s">
+      <c r="J121">
+        <v>22</v>
+      </c>
+      <c r="K121">
+        <v>13.4</v>
+      </c>
+      <c r="L121">
+        <v>12.9</v>
+      </c>
+      <c r="M121" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N121" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L121" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="122" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O121" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C122">
         <v>21.95</v>
       </c>
@@ -3843,17 +4050,26 @@
       <c r="I122">
         <v>-5.2901881248982043</v>
       </c>
-      <c r="J122" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K122" s="9" t="s">
+      <c r="J122">
+        <v>21.9</v>
+      </c>
+      <c r="K122">
+        <v>13.4</v>
+      </c>
+      <c r="L122">
+        <v>13</v>
+      </c>
+      <c r="M122" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N122" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L122" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="123" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O122" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C123">
         <v>16.3</v>
       </c>
@@ -3869,17 +4085,26 @@
       <c r="I123">
         <v>-4.7457805558256361</v>
       </c>
-      <c r="J123" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K123" s="9" t="s">
+      <c r="J123">
+        <v>22</v>
+      </c>
+      <c r="K123">
+        <v>13.3</v>
+      </c>
+      <c r="L123">
+        <v>13</v>
+      </c>
+      <c r="M123" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N123" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L123" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="124" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O123" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C124">
         <v>15.05</v>
       </c>
@@ -3895,17 +4120,26 @@
       <c r="I124">
         <v>-2.9178524704422135</v>
       </c>
-      <c r="J124" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K124" s="9" t="s">
+      <c r="J124">
+        <v>22</v>
+      </c>
+      <c r="K124">
+        <v>13.2</v>
+      </c>
+      <c r="L124">
+        <v>13</v>
+      </c>
+      <c r="M124" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N124" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L124" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="125" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O124" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C125">
         <v>13</v>
       </c>
@@ -3921,17 +4155,26 @@
       <c r="I125">
         <v>-5.5780663826707624</v>
       </c>
-      <c r="J125" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K125" s="9" t="s">
+      <c r="J125">
+        <v>22</v>
+      </c>
+      <c r="K125">
+        <v>13.350000000000001</v>
+      </c>
+      <c r="L125">
+        <v>13</v>
+      </c>
+      <c r="M125" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N125" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L125" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="126" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O125" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C126">
         <v>17.899999999999999</v>
       </c>
@@ -3947,17 +4190,26 @@
       <c r="I126">
         <v>-5.0888547229378265</v>
       </c>
-      <c r="J126" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K126" s="9" t="s">
+      <c r="J126">
+        <v>22</v>
+      </c>
+      <c r="K126">
+        <v>14.4</v>
+      </c>
+      <c r="L126">
+        <v>13</v>
+      </c>
+      <c r="M126" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N126" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L126" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="127" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O126" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C127">
         <v>13.3</v>
       </c>
@@ -3973,17 +4225,26 @@
       <c r="I127">
         <v>-9.2810036224946444</v>
       </c>
-      <c r="J127" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K127" s="9" t="s">
+      <c r="J127">
+        <v>21.9</v>
+      </c>
+      <c r="K127">
+        <v>13.7</v>
+      </c>
+      <c r="L127">
+        <v>13</v>
+      </c>
+      <c r="M127" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N127" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L127" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="128" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O127" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C128">
         <v>13.5</v>
       </c>
@@ -3999,17 +4260,26 @@
       <c r="I128">
         <v>-8.5964359549806542</v>
       </c>
-      <c r="J128" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K128" s="9" t="s">
+      <c r="J128">
+        <v>21.9</v>
+      </c>
+      <c r="K128">
+        <v>13.6</v>
+      </c>
+      <c r="L128">
+        <v>13</v>
+      </c>
+      <c r="M128" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N128" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L128" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="129" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="O128" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C129">
         <v>14.8</v>
       </c>
@@ -4025,19 +4295,28 @@
       <c r="I129">
         <v>-6.2613301682658271</v>
       </c>
-      <c r="J129" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K129" s="9" t="s">
+      <c r="J129">
+        <v>21.9</v>
+      </c>
+      <c r="K129">
+        <v>14.350000000000001</v>
+      </c>
+      <c r="L129">
+        <v>13</v>
+      </c>
+      <c r="M129" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N129" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L129" s="9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="130" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="K130" s="8"/>
-      <c r="L130" s="8"/>
+      <c r="O129" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="N130" s="8"/>
+      <c r="O130" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>